<commit_message>
Finishing up individual 1 work
</commit_message>
<xml_diff>
--- a/cyclonesFootball2019.xlsx
+++ b/cyclonesFootball2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xdai/GoogleDrive/Teaching/ISU/DS202 20S/crawl/cyclones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorturner/DS202/labs/ds202_lab4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5ED2AD-C8F2-B544-884A-72C902531BCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5EA8F2-C251-2B47-AEA9-F96DE4015027}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defensive" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Biography" sheetId="5" r:id="rId5"/>
     <sheet name="Glossaries" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -2254,7 +2254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K503"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
@@ -19875,8 +19875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L196"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>